<commit_message>
add high and low point for 1 day
</commit_message>
<xml_diff>
--- a/history/data_ticker_0503.xlsx
+++ b/history/data_ticker_0503.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavel.rostov\PycharmProjects\scrapyBotTrade\history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DCE012-9486-4884-8F16-51D5FEDF4E70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E5D1C4-4389-41CA-89FA-D492C412A872}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1209,7 +1209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1225,6 +1225,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1236,7 +1237,41 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1607,7 +1642,7 @@
   <dimension ref="A1:AD80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC16" sqref="AC16"/>
+      <selection activeCell="AH11" sqref="AH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,11 +1659,15 @@
         <v>35</v>
       </c>
       <c r="AA1" s="3">
-        <f>Z1/72</f>
+        <f>Z1/$U$2</f>
         <v>0.4861111111111111</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U2">
+        <f>SUBTOTAL(  2,A:A)</f>
+        <v>72</v>
+      </c>
       <c r="Y2" s="2" t="s">
         <v>353</v>
       </c>
@@ -1636,22 +1675,26 @@
         <v>12</v>
       </c>
       <c r="AA2" s="3">
-        <f t="shared" ref="AA2:AA5" si="0">Z2/72</f>
+        <f t="shared" ref="AA2:AA5" si="0">Z2/$U$2</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>345</v>
       </c>
       <c r="AD2" s="2">
-        <f>SUM(R7:R98)</f>
+        <f>SUBTOTAL( 9,R:R)</f>
         <v>2135.9199999999996</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K3" s="13">
+      <c r="K3" s="14">
         <v>44260</v>
       </c>
-      <c r="L3" s="14"/>
+      <c r="L3" s="15"/>
+      <c r="U3" s="7">
+        <f>SUBTOTAL(  2,V:V)</f>
+        <v>72</v>
+      </c>
       <c r="Y3" s="2" t="s">
         <v>354</v>
       </c>
@@ -1665,8 +1708,8 @@
       <c r="AC3" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="AD3" s="2">
-        <f>SUM(X7:X98)</f>
+      <c r="AD3" s="13">
+        <f>SUBTOTAL( 9,X:X)</f>
         <v>2183.5042124717152</v>
       </c>
     </row>
@@ -7109,49 +7152,70 @@
     <mergeCell ref="K3:L3"/>
   </mergeCells>
   <conditionalFormatting sqref="V80">
-    <cfRule type="cellIs" dxfId="8" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="21" operator="lessThan">
       <formula>0.005</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V80">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="20" operator="greaterThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V80">
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThan">
       <formula>0.02</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V80">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="between">
       <formula>0.006</formula>
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V7:V78">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
       <formula>1%</formula>
       <formula>1.5%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V7:V78">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
       <formula>0.015</formula>
       <formula>0.02</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V7:V78">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>0.02</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V7:V78">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>0.005</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
       <formula>0.005</formula>
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U3">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>0.005</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U3">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>0.012</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U3">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0.02</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U3">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>0.006</formula>
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>